<commit_message>
EventController Coverage Change Role Implemetation ModifyEventDetails not working
</commit_message>
<xml_diff>
--- a/build/classes/model/UserTestCases.xlsx
+++ b/build/classes/model/UserTestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Music\event_catering_management\test\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA21301-E909-4D0C-A564-60BD16A99B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89825D9-8EB2-41EF-8A24-184F3B4B0B8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="147">
   <si>
     <t>Test Case Number</t>
   </si>
@@ -812,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" workbookViewId="0">
-      <selection activeCell="P91" sqref="P91"/>
+    <sheetView tabSelected="1" topLeftCell="Q66" workbookViewId="0">
+      <selection activeCell="S86" sqref="S86:AC86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5133,12 +5133,6 @@
       <c r="D85" t="s">
         <v>49</v>
       </c>
-      <c r="E85" t="s">
-        <v>31</v>
-      </c>
-      <c r="F85" t="s">
-        <v>32</v>
-      </c>
       <c r="G85" t="s">
         <v>74</v>
       </c>
@@ -5146,25 +5140,41 @@
         <v>1001765834</v>
       </c>
       <c r="I85">
-        <v>4692580560</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K85">
-        <v>848</v>
-      </c>
-      <c r="L85" t="s">
-        <v>34</v>
-      </c>
-      <c r="M85" t="s">
-        <v>35</v>
-      </c>
-      <c r="N85" t="s">
-        <v>36</v>
-      </c>
+        <v>469258056</v>
+      </c>
+      <c r="J85" s="4"/>
       <c r="O85">
-        <v>76013</v>
+        <v>7601</v>
+      </c>
+      <c r="P85" t="s">
+        <v>39</v>
+      </c>
+      <c r="S85" t="s">
+        <v>90</v>
+      </c>
+      <c r="T85" t="s">
+        <v>101</v>
+      </c>
+      <c r="W85" t="s">
+        <v>66</v>
+      </c>
+      <c r="X85" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z85" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA85" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC85" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.3">
@@ -5174,44 +5184,57 @@
       <c r="B86" t="s">
         <v>115</v>
       </c>
-      <c r="C86" t="s">
-        <v>44</v>
-      </c>
       <c r="D86" t="s">
         <v>49</v>
       </c>
-      <c r="E86" t="s">
-        <v>31</v>
-      </c>
-      <c r="F86" t="s">
-        <v>32</v>
-      </c>
       <c r="G86" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H86" s="3">
         <v>1001765834</v>
       </c>
       <c r="I86">
-        <v>4692580560</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K86">
-        <v>848</v>
-      </c>
-      <c r="L86" t="s">
-        <v>34</v>
-      </c>
-      <c r="M86" t="s">
-        <v>35</v>
-      </c>
-      <c r="N86" t="s">
-        <v>36</v>
-      </c>
+        <v>469258056</v>
+      </c>
+      <c r="J86" s="4"/>
       <c r="O86">
-        <v>76013</v>
+        <v>7601</v>
+      </c>
+      <c r="P86" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>37</v>
+      </c>
+      <c r="S86" t="s">
+        <v>90</v>
+      </c>
+      <c r="T86" t="s">
+        <v>101</v>
+      </c>
+      <c r="U86" t="s">
+        <v>87</v>
+      </c>
+      <c r="W86" t="s">
+        <v>66</v>
+      </c>
+      <c r="X86" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z86" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA86" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC86" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:29" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Profile Update All Users and Change Role Scenario
</commit_message>
<xml_diff>
--- a/build/classes/model/UserTestCases.xlsx
+++ b/build/classes/model/UserTestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Music\event_catering_management\test\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89825D9-8EB2-41EF-8A24-184F3B4B0B8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBCF7BE-23E9-4AFF-ACA8-188A1B8B043A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="148">
   <si>
     <t>Test Case Number</t>
   </si>
@@ -466,6 +466,9 @@
   </si>
   <si>
     <t>Incorrect password</t>
+  </si>
+  <si>
+    <t>changeRole</t>
   </si>
 </sst>
 </file>
@@ -810,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE91"/>
+  <dimension ref="A1:AE92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q66" workbookViewId="0">
-      <selection activeCell="S86" sqref="S86:AC86"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5203,9 +5206,6 @@
       <c r="P86" t="s">
         <v>39</v>
       </c>
-      <c r="Q86" t="s">
-        <v>37</v>
-      </c>
       <c r="S86" t="s">
         <v>90</v>
       </c>
@@ -5490,6 +5490,59 @@
       </c>
       <c r="R91" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="92" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>89</v>
+      </c>
+      <c r="B92" t="s">
+        <v>147</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D92" t="s">
+        <v>118</v>
+      </c>
+      <c r="E92" t="s">
+        <v>31</v>
+      </c>
+      <c r="F92" t="s">
+        <v>32</v>
+      </c>
+      <c r="G92" t="s">
+        <v>75</v>
+      </c>
+      <c r="H92">
+        <v>1001765834</v>
+      </c>
+      <c r="I92">
+        <v>4692580560</v>
+      </c>
+      <c r="J92" t="s">
+        <v>33</v>
+      </c>
+      <c r="K92">
+        <v>848</v>
+      </c>
+      <c r="L92" t="s">
+        <v>34</v>
+      </c>
+      <c r="M92" t="s">
+        <v>35</v>
+      </c>
+      <c r="N92" t="s">
+        <v>36</v>
+      </c>
+      <c r="O92">
+        <v>76013</v>
+      </c>
+      <c r="P92" t="s">
+        <v>39</v>
+      </c>
+      <c r="U92" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>